<commit_message>
next chapter on going
</commit_message>
<xml_diff>
--- a/Final_Project/Material_for_Documentation/Losses for different types of Cycle GAN.xlsx
+++ b/Final_Project/Material_for_Documentation/Losses for different types of Cycle GAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7febc520ade5fca9/Master_Cognitive_Computing/1_Semester/IANN_group30/Final_project/Material_for_Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF812E23-ACB7-4FBB-B779-6756D1A3851D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{FF812E23-ACB7-4FBB-B779-6756D1A3851D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A38DB5B8-41D4-403D-B9A9-212F289E6061}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
               <a:rPr lang="en-GB" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>for different types of Cycle GAN</a:t>
+              <a:t>for different types of CycleGAN</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1600" b="1">
               <a:solidFill>
@@ -925,7 +925,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t> GAN</a:t>
+              <a:t>GAN</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB" sz="1600" b="1">
               <a:solidFill>
@@ -935,6 +935,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16308314550214639"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2739,9 +2747,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2771,13 +2779,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>167639</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3104,8 +3112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>